<commit_message>
moved files/edited raw files
</commit_message>
<xml_diff>
--- a/BacillusData/Stamm185/metadata.xlsx
+++ b/BacillusData/Stamm185/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusDaten\Stamm185\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusData\Stamm185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A579D4-DE2A-4AD5-86A6-DF0ACFE190F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA3DA2F-136F-439E-98FD-965926C9FAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="1740" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Experiment</t>
   </si>
@@ -84,67 +84,73 @@
     <t>F3</t>
   </si>
   <si>
+    <t>Sim_end</t>
+  </si>
+  <si>
+    <t>F_end</t>
+  </si>
+  <si>
+    <t>feed_%_to_mL</t>
+  </si>
+  <si>
+    <t>feed_rate_mL_to_g</t>
+  </si>
+  <si>
+    <t>dd.mm.yyyy hh:mm</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>OD_to_CDW_factor</t>
+  </si>
+  <si>
+    <t>g/L</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>lpm</t>
+  </si>
+  <si>
+    <t>gL/OD</t>
+  </si>
+  <si>
+    <t>g/mL</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>cNH3</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>no sample volume, offline Measurments = double measurments</t>
+  </si>
+  <si>
+    <t>offline Measurments = triple measurments</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>mX0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mL/%/min </t>
+  </si>
+  <si>
+    <t>cP0</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
     <t>mP0</t>
-  </si>
-  <si>
-    <t>Sim_end</t>
-  </si>
-  <si>
-    <t>F_end</t>
-  </si>
-  <si>
-    <t>feed_%_to_mL</t>
-  </si>
-  <si>
-    <t>feed_rate_mL_to_g</t>
-  </si>
-  <si>
-    <t>dd.mm.yyyy hh:mm</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>OD_to_CDW_factor</t>
-  </si>
-  <si>
-    <t>g/L</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>lpm</t>
-  </si>
-  <si>
-    <t>gL/OD</t>
-  </si>
-  <si>
-    <t>mL/%</t>
-  </si>
-  <si>
-    <t>g/mL</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>cNH3</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>no sample volume, offline Measurments = double measurments</t>
-  </si>
-  <si>
-    <t>offline Measurments = triple measurments</t>
-  </si>
-  <si>
-    <t>mg/L</t>
-  </si>
-  <si>
-    <t>mX0</t>
   </si>
 </sst>
 </file>
@@ -237,8 +243,8 @@
     <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,9 +542,10 @@
     <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="5"/>
     <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,10 +559,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -564,7 +571,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -573,13 +580,13 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
@@ -591,73 +598,79 @@
         <v>9</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
       <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>30</v>
-      </c>
       <c r="R2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -717,11 +730,15 @@
       <c r="S3" s="5">
         <v>0</v>
       </c>
-      <c r="T3" t="s">
-        <v>33</v>
+      <c r="T3" s="16">
+        <f>S3*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -778,14 +795,18 @@
       <c r="R4" s="5">
         <v>184.61</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4">
         <v>5.24</v>
       </c>
-      <c r="T4" t="s">
-        <v>33</v>
+      <c r="T4" s="16">
+        <f t="shared" ref="T4:T7" si="1">S4*0.5</f>
+        <v>2.62</v>
+      </c>
+      <c r="U4" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -845,11 +866,15 @@
       <c r="S5" s="9">
         <v>1.0241379310344827</v>
       </c>
-      <c r="T5" t="s">
-        <v>34</v>
+      <c r="T5" s="16">
+        <f t="shared" si="1"/>
+        <v>0.51206896551724135</v>
+      </c>
+      <c r="U5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -906,14 +931,18 @@
       <c r="R6" s="5">
         <v>184.61</v>
       </c>
-      <c r="S6" s="16">
+      <c r="S6" s="17">
         <v>10.6206896551724</v>
       </c>
-      <c r="T6" t="s">
-        <v>34</v>
+      <c r="T6" s="16">
+        <f t="shared" si="1"/>
+        <v>5.3103448275862002</v>
+      </c>
+      <c r="U6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -973,11 +1002,15 @@
       <c r="S7" s="9">
         <v>0.44137931034482758</v>
       </c>
-      <c r="T7" t="s">
-        <v>34</v>
+      <c r="T7" s="16">
+        <f t="shared" si="1"/>
+        <v>0.22068965517241379</v>
+      </c>
+      <c r="U7" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -990,9 +1023,10 @@
       <c r="O8" s="9"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="17"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1005,7 +1039,8 @@
       <c r="O9" s="9"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="5"/>
-      <c r="S9" s="17"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
incorporated the viability factor
</commit_message>
<xml_diff>
--- a/BacillusData/Stamm185/metadata.xlsx
+++ b/BacillusData/Stamm185/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusData\Stamm185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A6A55A-ED29-4D51-B945-4F01531E4BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794FE8FE-FC57-4356-BDB0-E9BE79FE3D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="5535" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Experiment</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>mX0_ohne_viab_f</t>
   </si>
 </sst>
 </file>
@@ -531,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,17 +545,17 @@
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="5"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="11.5703125" customWidth="1"/>
-    <col min="22" max="22" width="9" customWidth="1"/>
+    <col min="8" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="5"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.5703125" customWidth="1"/>
+    <col min="24" max="24" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,49 +581,55 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -646,44 +655,50 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="2"/>
+      <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -712,49 +727,56 @@
         <f>H3*0.5</f>
         <v>0.01</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="10">
+        <v>1</v>
+      </c>
+      <c r="K3" s="10">
+        <f>I3*J3</f>
+        <v>0.01</v>
+      </c>
+      <c r="L3" s="9">
         <v>27.560040253447639</v>
       </c>
-      <c r="K3" s="11">
-        <f>J3*0.5</f>
+      <c r="M3" s="11">
+        <f>L3*0.5</f>
         <v>13.780020126723819</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>0.3669</v>
       </c>
-      <c r="M3" s="5">
+      <c r="O3" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="N3" s="5">
+      <c r="P3" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="O3" s="9">
+      <c r="Q3" s="9">
         <v>150</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>0.5</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>37</v>
       </c>
-      <c r="R3" s="5">
+      <c r="T3" s="5">
         <v>184.61</v>
       </c>
-      <c r="S3" s="5">
+      <c r="U3" s="5">
         <v>0</v>
       </c>
-      <c r="T3" s="16">
-        <f>S3*0.5</f>
+      <c r="V3" s="16">
+        <f>U3*0.5</f>
         <v>0</v>
       </c>
-      <c r="U3" s="16">
+      <c r="W3" s="16">
         <v>1</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -780,52 +802,59 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="I4" s="10">
-        <f t="shared" ref="I4:K7" si="0">H4*0.5</f>
+        <f t="shared" ref="I4:M7" si="0">H4*0.5</f>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="10">
+        <v>0.46850000000000003</v>
+      </c>
+      <c r="K4" s="10">
+        <f t="shared" ref="K4:K7" si="1">I4*J4</f>
+        <v>8.4329999999999995E-3</v>
+      </c>
+      <c r="L4" s="9">
         <v>19.608350430319199</v>
       </c>
-      <c r="K4" s="11">
+      <c r="M4" s="11">
         <f t="shared" si="0"/>
         <v>9.8041752151595993</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>0.3669</v>
       </c>
-      <c r="M4" s="5">
+      <c r="O4" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="N4" s="5">
+      <c r="P4" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="O4" s="9">
+      <c r="Q4" s="9">
         <v>150</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>0.5</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>37</v>
       </c>
-      <c r="R4" s="5">
+      <c r="T4" s="5">
         <v>184.61</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>5.24</v>
       </c>
-      <c r="T4" s="16">
-        <f t="shared" ref="T4:T7" si="1">S4*0.5</f>
+      <c r="V4" s="16">
+        <f t="shared" ref="V4:V7" si="2">U4*0.5</f>
         <v>2.62</v>
       </c>
-      <c r="U4" s="16">
+      <c r="W4" s="16">
         <v>1</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -854,49 +883,56 @@
         <f t="shared" si="0"/>
         <v>4.0028790000000002E-2</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="10">
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="K5" s="10">
+        <f t="shared" si="1"/>
+        <v>4.2750747720000006E-3</v>
+      </c>
+      <c r="L5" s="9">
         <v>27.369118762743817</v>
       </c>
-      <c r="K5" s="11">
+      <c r="M5" s="11">
         <f t="shared" si="0"/>
         <v>13.684559381371908</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>0.3669</v>
       </c>
-      <c r="M5" s="5">
+      <c r="O5" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="N5" s="5">
+      <c r="P5" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="O5" s="9">
+      <c r="Q5" s="9">
         <v>303.51</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>0.5</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>37</v>
       </c>
-      <c r="R5" s="5">
+      <c r="T5" s="5">
         <v>184.61</v>
       </c>
-      <c r="S5" s="9">
+      <c r="U5" s="9">
         <v>1.0241379310344827</v>
       </c>
-      <c r="T5" s="16">
-        <f t="shared" si="1"/>
+      <c r="V5" s="16">
+        <f t="shared" si="2"/>
         <v>0.51206896551724135</v>
       </c>
-      <c r="U5" s="16">
+      <c r="W5" s="16">
         <v>1</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -925,49 +961,56 @@
         <f t="shared" si="0"/>
         <v>2.1885584999999999E-2</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="10">
+        <v>0.2122</v>
+      </c>
+      <c r="K6" s="10">
+        <f t="shared" si="1"/>
+        <v>4.6441211370000001E-3</v>
+      </c>
+      <c r="L6" s="9">
         <v>32.781673628850491</v>
       </c>
-      <c r="K6" s="11">
+      <c r="M6" s="11">
         <f t="shared" si="0"/>
         <v>16.390836814425246</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>0.3669</v>
       </c>
-      <c r="M6" s="5">
+      <c r="O6" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="N6" s="5">
+      <c r="P6" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="O6" s="9">
+      <c r="Q6" s="9">
         <v>335.72072126220888</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>0.5</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>37</v>
       </c>
-      <c r="R6" s="5">
+      <c r="T6" s="5">
         <v>184.61</v>
       </c>
-      <c r="S6" s="17">
+      <c r="U6" s="17">
         <v>10.6206896551724</v>
       </c>
-      <c r="T6" s="16">
-        <f t="shared" si="1"/>
+      <c r="V6" s="16">
+        <f t="shared" si="2"/>
         <v>5.3103448275862002</v>
       </c>
-      <c r="U6" s="16">
+      <c r="W6" s="16">
         <v>1</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -996,49 +1039,56 @@
         <f t="shared" si="0"/>
         <v>2.6948804999999999E-2</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="15">
+        <v>0.4965</v>
+      </c>
+      <c r="K7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.3380081682499999E-2</v>
+      </c>
+      <c r="L7" s="14">
         <v>30.541769797145008</v>
       </c>
-      <c r="K7" s="12">
+      <c r="M7" s="12">
         <f t="shared" si="0"/>
         <v>15.270884898572504</v>
       </c>
-      <c r="L7" s="3">
+      <c r="N7" s="3">
         <v>0.3669</v>
       </c>
-      <c r="M7" s="6">
+      <c r="O7" s="6">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="N7" s="6">
+      <c r="P7" s="6">
         <v>1.1399999999999999</v>
       </c>
-      <c r="O7" s="14">
+      <c r="Q7" s="14">
         <v>336.59095416979716</v>
       </c>
-      <c r="P7" s="3">
+      <c r="R7" s="3">
         <v>0.5</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="S7" s="3">
         <v>37</v>
       </c>
-      <c r="R7" s="6">
+      <c r="T7" s="6">
         <v>184.61</v>
       </c>
-      <c r="S7" s="9">
+      <c r="U7" s="9">
         <v>0.44137931034482758</v>
       </c>
-      <c r="T7" s="16">
-        <f t="shared" si="1"/>
+      <c r="V7" s="16">
+        <f t="shared" si="2"/>
         <v>0.22068965517241379</v>
       </c>
-      <c r="U7" s="16">
+      <c r="W7" s="16">
         <v>1</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1046,16 +1096,18 @@
       <c r="F8" s="1"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="11"/>
-      <c r="O8" s="9"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="11"/>
+      <c r="Q8" s="9"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="5"/>
       <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1063,14 +1115,16 @@
       <c r="F9" s="1"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="11"/>
-      <c r="O9" s="9"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="11"/>
+      <c r="Q9" s="9"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="5"/>
       <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed correlation factor pump
</commit_message>
<xml_diff>
--- a/BacillusData/Stamm185/metadata.xlsx
+++ b/BacillusData/Stamm185/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusData\Stamm185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794FE8FE-FC57-4356-BDB0-E9BE79FE3D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A207BE-2908-40BD-AEC6-53CF35B588D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
         <v>40</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
         <v>23</v>
@@ -748,7 +748,7 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="P3" s="5">
-        <v>1.1399999999999999</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="Q3" s="9">
         <v>150</v>
@@ -809,7 +809,7 @@
         <v>0.46850000000000003</v>
       </c>
       <c r="K4" s="10">
-        <f t="shared" ref="K4:K7" si="1">I4*J4</f>
+        <f t="shared" ref="K4:K6" si="1">I4*J4</f>
         <v>8.4329999999999995E-3</v>
       </c>
       <c r="L4" s="9">
@@ -826,7 +826,7 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="P4" s="5">
-        <v>1.1399999999999999</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="Q4" s="9">
         <v>150</v>
@@ -904,7 +904,7 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="P5" s="5">
-        <v>1.1399999999999999</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="Q5" s="9">
         <v>303.51</v>
@@ -982,7 +982,7 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="P6" s="5">
-        <v>1.1399999999999999</v>
+        <v>1.1639999999999999</v>
       </c>
       <c r="Q6" s="9">
         <v>335.72072126220888</v>
@@ -1043,7 +1043,7 @@
         <v>0.4965</v>
       </c>
       <c r="K7" s="15">
-        <f t="shared" si="1"/>
+        <f>I7*J7</f>
         <v>1.3380081682499999E-2</v>
       </c>
       <c r="L7" s="14">
@@ -1057,10 +1057,10 @@
         <v>0.3669</v>
       </c>
       <c r="O7" s="6">
-        <v>8.6400000000000005E-2</v>
-      </c>
-      <c r="P7" s="6">
-        <v>1.1399999999999999</v>
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="P7" s="5">
+        <v>1.1639999999999999</v>
       </c>
       <c r="Q7" s="14">
         <v>336.59095416979716</v>

</xml_diff>

<commit_message>
added rectangular to graphs indicating which timeframe was considert for simulation
</commit_message>
<xml_diff>
--- a/BacillusData/Stamm185/metadata.xlsx
+++ b/BacillusData/Stamm185/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusData\Stamm185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CE0F8B-70B9-4AFE-95E6-A26CD7B89AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247BB7D0-CC2F-4E82-9A87-52760F12D31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2775" yWindow="4515" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +712,7 @@
         <v>44518.378472222219</v>
       </c>
       <c r="E3" s="1">
-        <v>44518.742523148147</v>
+        <v>44518.750162037039</v>
       </c>
       <c r="F3" s="1">
         <v>44519.396574074075</v>
@@ -869,7 +869,7 @@
         <v>44538.417361111111</v>
       </c>
       <c r="E5" s="1">
-        <v>44539.07402777778</v>
+        <v>44539.365694444445</v>
       </c>
       <c r="F5" s="1">
         <v>44540.415277777778</v>
@@ -1027,7 +1027,7 @@
         <v>44545.447222222225</v>
       </c>
       <c r="E7" s="4">
-        <v>44546.270844907405</v>
+        <v>44546.395844907405</v>
       </c>
       <c r="F7" s="1">
         <v>44547.402083333334</v>

</xml_diff>